<commit_message>
- added a Missions tab to Demo.xlsx - task-service reading data from Demo.xlsx - timeline no longer needs to parse data as an "#inst" is returned from the server
</commit_message>
<xml_diff>
--- a/resources/public/excel/Demo.xlsx
+++ b/resources/public/excel/Demo.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unencrypted Folder\9102Demo Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wassech\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SCN_NETWORK_CARRIER_VW" sheetId="2" r:id="rId1"/>
     <sheet name="LINK_COMPOSITE_PRED" sheetId="3" r:id="rId2"/>
     <sheet name="Terminals" sheetId="1" r:id="rId3"/>
     <sheet name="Beams" sheetId="5" r:id="rId4"/>
+    <sheet name="Missions" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5155" uniqueCount="3827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5189" uniqueCount="3846">
   <si>
     <t>{009CE8FE-B526-42F9-89A2-F117BF975AF0}</t>
   </si>
@@ -11508,12 +11509,72 @@
   </si>
   <si>
     <t>NWT - Darwin</t>
+  </si>
+  <si>
+    <t>Mission-002</t>
+  </si>
+  <si>
+    <t>Dulles</t>
+  </si>
+  <si>
+    <t>Mission-001</t>
+  </si>
+  <si>
+    <t>Mission-003</t>
+  </si>
+  <si>
+    <t>Mission-004</t>
+  </si>
+  <si>
+    <t>Mission-005</t>
+  </si>
+  <si>
+    <t>Mission-006</t>
+  </si>
+  <si>
+    <t>Mission-007</t>
+  </si>
+  <si>
+    <t>Mission-008</t>
+  </si>
+  <si>
+    <t>Mission-009</t>
+  </si>
+  <si>
+    <t>Mission-010</t>
+  </si>
+  <si>
+    <t>Mission-011</t>
+  </si>
+  <si>
+    <t>Mission-012</t>
+  </si>
+  <si>
+    <t>Mission-013</t>
+  </si>
+  <si>
+    <t>Mission-014</t>
+  </si>
+  <si>
+    <t>Mission-015</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Start</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11552,13 +11613,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -59073,7 +59135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -59267,13 +59329,253 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3803</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3843</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3845</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3844</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3829</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3827</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C3" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D3" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3830</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C4" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D4" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3831</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3821</v>
+      </c>
+      <c r="C5" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D5" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3832</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3825</v>
+      </c>
+      <c r="C6" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D6" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3833</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3828</v>
+      </c>
+      <c r="C7" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D7" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3834</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D8" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3835</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C9" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D9" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3836</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C10" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D10" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3837</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3821</v>
+      </c>
+      <c r="C11" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3825</v>
+      </c>
+      <c r="C12" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3839</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3828</v>
+      </c>
+      <c r="C13" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3840</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3820</v>
+      </c>
+      <c r="C14" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D14" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3841</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C15" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3842</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3819</v>
+      </c>
+      <c r="C16" s="6">
+        <v>43864.541666666664</v>
+      </c>
+      <c r="D16" s="6">
+        <v>44190.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D007B09EFB8E04990DCD0CE29ED7BFA" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cead2ce28f5b86dc332205d79569db33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -59387,7 +59689,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -59396,22 +59698,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D0860C-F54E-4E5F-9EF1-B43D49FC0784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D840BE61-2D2D-4AD5-AFD8-2E39857E67FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59427,10 +59720,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3880DD5E-8917-42BB-AA42-9F04DAC43F18}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D0860C-F54E-4E5F-9EF1-B43D49FC0784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- pulling beam-layer data from the beam-location-service
</commit_message>
<xml_diff>
--- a/resources/public/excel/Demo.xlsx
+++ b/resources/public/excel/Demo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wassech\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unencrypted Folder\9102Demo Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SCN_NETWORK_CARRIER_VW" sheetId="2" r:id="rId1"/>
@@ -59135,12 +59135,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -59175,7 +59176,7 @@
         <v>-81.379233999999997</v>
       </c>
       <c r="D2">
-        <v>75000</v>
+        <v>750000</v>
       </c>
       <c r="E2" t="s">
         <v>3818</v>
@@ -59195,7 +59196,7 @@
         <v>-99.174099999999996</v>
       </c>
       <c r="D3">
-        <v>150000</v>
+        <v>1500000</v>
       </c>
       <c r="E3" t="s">
         <v>3816</v>
@@ -59215,7 +59216,7 @@
         <v>134.3887</v>
       </c>
       <c r="D4">
-        <v>200000</v>
+        <v>2000000</v>
       </c>
       <c r="E4" t="s">
         <v>3816</v>
@@ -59235,7 +59236,7 @@
         <v>-81.379233999999997</v>
       </c>
       <c r="D5">
-        <v>22500</v>
+        <v>225000</v>
       </c>
       <c r="E5" t="s">
         <v>3817</v>
@@ -59255,7 +59256,7 @@
         <v>-117.16108699999999</v>
       </c>
       <c r="D6">
-        <v>22500</v>
+        <v>225000</v>
       </c>
       <c r="E6" t="s">
         <v>3817</v>
@@ -59275,7 +59276,7 @@
         <v>149.13</v>
       </c>
       <c r="D7">
-        <v>22500</v>
+        <v>225000</v>
       </c>
       <c r="E7" t="s">
         <v>3817</v>
@@ -59295,7 +59296,7 @@
         <v>114.607513</v>
       </c>
       <c r="D8">
-        <v>22500</v>
+        <v>225000</v>
       </c>
       <c r="E8" t="s">
         <v>3817</v>
@@ -59315,7 +59316,7 @@
         <v>130.88300000000001</v>
       </c>
       <c r="D9">
-        <v>37560</v>
+        <v>375600</v>
       </c>
       <c r="E9" t="s">
         <v>3818</v>
@@ -59333,7 +59334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -59576,6 +59577,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003D007B09EFB8E04990DCD0CE29ED7BFA" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cead2ce28f5b86dc332205d79569db33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -59689,22 +59705,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D0860C-F54E-4E5F-9EF1-B43D49FC0784}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3880DD5E-8917-42BB-AA42-9F04DAC43F18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D840BE61-2D2D-4AD5-AFD8-2E39857E67FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59718,27 +59742,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3880DD5E-8917-42BB-AA42-9F04DAC43F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D0860C-F54E-4E5F-9EF1-B43D49FC0784}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- changes to the structure of several worksheet in the Demo.xlsx file (signal-path still incorrect) - show beam name on the layer - sort task and signal-path data at the server
</commit_message>
<xml_diff>
--- a/resources/public/excel/Demo.xlsx
+++ b/resources/public/excel/Demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unencrypted Folder\9102Demo Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wassech\Desktop\Area51\Blackhammer\9102 Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5189" uniqueCount="3846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5190" uniqueCount="3839">
   <si>
     <t>{009CE8FE-B526-42F9-89A2-F117BF975AF0}</t>
   </si>
@@ -11454,30 +11454,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>b-1</t>
-  </si>
-  <si>
-    <t>b-2</t>
-  </si>
-  <si>
-    <t>b-3</t>
-  </si>
-  <si>
-    <t>b-4</t>
-  </si>
-  <si>
-    <t>b-5</t>
-  </si>
-  <si>
-    <t>b-6</t>
-  </si>
-  <si>
-    <t>b-7</t>
-  </si>
-  <si>
-    <t>b-8</t>
-  </si>
-  <si>
     <t>Broadcast</t>
   </si>
   <si>
@@ -11566,6 +11542,9 @@
   </si>
   <si>
     <t>Start</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -11613,7 +11592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -11621,6 +11600,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -59133,200 +59114,228 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3807</v>
+      </c>
+      <c r="B1" t="s">
         <v>3803</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3804</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3805</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3806</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3807</v>
       </c>
-      <c r="F1" t="s">
-        <v>3824</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>28.538336000000001</v>
+      </c>
+      <c r="D2">
+        <v>-81.379233999999997</v>
+      </c>
+      <c r="E2" s="7">
+        <v>325000</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3810</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>40.1188</v>
+      </c>
+      <c r="D3">
+        <v>-99.174099999999996</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F3" t="s">
         <v>3808</v>
       </c>
-      <c r="B2">
+      <c r="G3" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>-24.683700000000002</v>
+      </c>
+      <c r="D4">
+        <v>134.3887</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3808</v>
+      </c>
+      <c r="G4" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>28.538336000000001</v>
       </c>
-      <c r="C2">
+      <c r="D5">
         <v>-81.379233999999997</v>
       </c>
-      <c r="D2">
-        <v>750000</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="E5" s="7">
+        <v>111000</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3809</v>
+      </c>
+      <c r="G5" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>32.715736</v>
+      </c>
+      <c r="D6">
+        <v>-117.16108699999999</v>
+      </c>
+      <c r="E6" s="7">
+        <v>111000</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3809</v>
+      </c>
+      <c r="G6" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>-35.280900000000003</v>
+      </c>
+      <c r="D7">
+        <v>149.13</v>
+      </c>
+      <c r="E7" s="7">
+        <v>111000</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3809</v>
+      </c>
+      <c r="G7" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>-28.782387</v>
+      </c>
+      <c r="D8">
+        <v>114.607513</v>
+      </c>
+      <c r="E8" s="7">
+        <v>111000</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3809</v>
+      </c>
+      <c r="G8" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>-12.633699999999999</v>
+      </c>
+      <c r="D9">
+        <v>130.88300000000001</v>
+      </c>
+      <c r="E9" s="7">
+        <v>145600</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3810</v>
+      </c>
+      <c r="G9" t="s">
         <v>3818</v>
-      </c>
-      <c r="F2" t="s">
-        <v>3819</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3809</v>
-      </c>
-      <c r="B3">
-        <v>40.1188</v>
-      </c>
-      <c r="C3">
-        <v>-99.174099999999996</v>
-      </c>
-      <c r="D3">
-        <v>1500000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3816</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3822</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3810</v>
-      </c>
-      <c r="B4">
-        <v>-24.683700000000002</v>
-      </c>
-      <c r="C4">
-        <v>134.3887</v>
-      </c>
-      <c r="D4">
-        <v>2000000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3816</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3823</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3811</v>
-      </c>
-      <c r="B5">
-        <v>28.538336000000001</v>
-      </c>
-      <c r="C5">
-        <v>-81.379233999999997</v>
-      </c>
-      <c r="D5">
-        <v>225000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>3817</v>
-      </c>
-      <c r="F5" t="s">
-        <v>3819</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3812</v>
-      </c>
-      <c r="B6">
-        <v>32.715736</v>
-      </c>
-      <c r="C6">
-        <v>-117.16108699999999</v>
-      </c>
-      <c r="D6">
-        <v>225000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>3817</v>
-      </c>
-      <c r="F6" t="s">
-        <v>3820</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3813</v>
-      </c>
-      <c r="B7">
-        <v>-35.280900000000003</v>
-      </c>
-      <c r="C7">
-        <v>149.13</v>
-      </c>
-      <c r="D7">
-        <v>225000</v>
-      </c>
-      <c r="E7" t="s">
-        <v>3817</v>
-      </c>
-      <c r="F7" t="s">
-        <v>3821</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3814</v>
-      </c>
-      <c r="B8">
-        <v>-28.782387</v>
-      </c>
-      <c r="C8">
-        <v>114.607513</v>
-      </c>
-      <c r="D8">
-        <v>225000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3817</v>
-      </c>
-      <c r="F8" t="s">
-        <v>3825</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3815</v>
-      </c>
-      <c r="B9">
-        <v>-12.633699999999999</v>
-      </c>
-      <c r="C9">
-        <v>130.88300000000001</v>
-      </c>
-      <c r="D9">
-        <v>375600</v>
-      </c>
-      <c r="E9" t="s">
-        <v>3818</v>
-      </c>
-      <c r="F9" t="s">
-        <v>3826</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -59335,15 +59344,15 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13" style="8" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -59351,21 +59360,21 @@
         <v>3803</v>
       </c>
       <c r="B1" t="s">
-        <v>3843</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3845</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3844</v>
+        <v>3835</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>3837</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3836</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3829</v>
+        <v>3821</v>
       </c>
       <c r="B2" t="s">
-        <v>3819</v>
+        <v>3811</v>
       </c>
       <c r="C2" s="6">
         <v>43864.541666666664</v>
@@ -59376,52 +59385,52 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3827</v>
+        <v>3819</v>
       </c>
       <c r="B3" t="s">
-        <v>3819</v>
+        <v>3811</v>
       </c>
       <c r="C3" s="6">
-        <v>43864.541666666664</v>
+        <v>43960.541666666664</v>
       </c>
       <c r="D3" s="6">
-        <v>44190.5</v>
+        <v>44037.5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3830</v>
+        <v>3822</v>
       </c>
       <c r="B4" t="s">
-        <v>3820</v>
+        <v>3812</v>
       </c>
       <c r="C4" s="6">
         <v>43864.541666666664</v>
       </c>
       <c r="D4" s="6">
-        <v>44190.5</v>
+        <v>43984.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3831</v>
+        <v>3823</v>
       </c>
       <c r="B5" t="s">
-        <v>3821</v>
+        <v>3813</v>
       </c>
       <c r="C5" s="6">
-        <v>43864.541666666664</v>
+        <v>43833.541666666664</v>
       </c>
       <c r="D5" s="6">
-        <v>44190.5</v>
+        <v>43886.5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3832</v>
+        <v>3824</v>
       </c>
       <c r="B6" t="s">
-        <v>3825</v>
+        <v>3817</v>
       </c>
       <c r="C6" s="6">
         <v>43864.541666666664</v>
@@ -59432,52 +59441,52 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3833</v>
+        <v>3825</v>
       </c>
       <c r="B7" t="s">
-        <v>3828</v>
+        <v>3820</v>
       </c>
       <c r="C7" s="6">
-        <v>43864.541666666664</v>
+        <v>43960.541666666664</v>
       </c>
       <c r="D7" s="6">
-        <v>44190.5</v>
+        <v>44037.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3834</v>
+        <v>3826</v>
       </c>
       <c r="B8" t="s">
-        <v>3820</v>
+        <v>3812</v>
       </c>
       <c r="C8" s="6">
         <v>43864.541666666664</v>
       </c>
       <c r="D8" s="6">
-        <v>44190.5</v>
+        <v>43984.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3835</v>
+        <v>3827</v>
       </c>
       <c r="B9" t="s">
-        <v>3819</v>
+        <v>3811</v>
       </c>
       <c r="C9" s="6">
-        <v>43864.541666666664</v>
+        <v>43833.541666666664</v>
       </c>
       <c r="D9" s="6">
-        <v>44190.5</v>
+        <v>43886.5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3836</v>
+        <v>3828</v>
       </c>
       <c r="B10" t="s">
-        <v>3820</v>
+        <v>3812</v>
       </c>
       <c r="C10" s="6">
         <v>43864.541666666664</v>
@@ -59488,52 +59497,52 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>3837</v>
+        <v>3829</v>
       </c>
       <c r="B11" t="s">
-        <v>3821</v>
+        <v>3813</v>
       </c>
       <c r="C11" s="6">
-        <v>43864.541666666664</v>
+        <v>43960.541666666664</v>
       </c>
       <c r="D11" s="6">
-        <v>44190.5</v>
+        <v>44037.5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>3838</v>
+        <v>3830</v>
       </c>
       <c r="B12" t="s">
-        <v>3825</v>
+        <v>3817</v>
       </c>
       <c r="C12" s="6">
         <v>43864.541666666664</v>
       </c>
       <c r="D12" s="6">
-        <v>44190.5</v>
+        <v>43984.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3839</v>
+        <v>3831</v>
       </c>
       <c r="B13" t="s">
-        <v>3828</v>
+        <v>3820</v>
       </c>
       <c r="C13" s="6">
-        <v>43864.541666666664</v>
+        <v>43833.541666666664</v>
       </c>
       <c r="D13" s="6">
-        <v>44190.5</v>
+        <v>43886.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3840</v>
+        <v>3832</v>
       </c>
       <c r="B14" t="s">
-        <v>3820</v>
+        <v>3812</v>
       </c>
       <c r="C14" s="6">
         <v>43864.541666666664</v>
@@ -59544,30 +59553,30 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>3841</v>
+        <v>3833</v>
       </c>
       <c r="B15" t="s">
-        <v>3819</v>
+        <v>3811</v>
       </c>
       <c r="C15" s="6">
-        <v>43864.541666666664</v>
+        <v>43960.541666666664</v>
       </c>
       <c r="D15" s="6">
-        <v>44190.5</v>
+        <v>44037.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>3842</v>
+        <v>3834</v>
       </c>
       <c r="B16" t="s">
-        <v>3819</v>
+        <v>3811</v>
       </c>
       <c r="C16" s="6">
-        <v>43864.541666666664</v>
+        <v>44077.541666666664</v>
       </c>
       <c r="D16" s="6">
-        <v>44190.5</v>
+        <v>44349.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- removed ":minWidth" form arearange-chart - updated beam locations and radii in Demo.xlsx
</commit_message>
<xml_diff>
--- a/resources/public/excel/Demo.xlsx
+++ b/resources/public/excel/Demo.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27015" windowHeight="17670" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SCN_NETWORK_CARRIER_VW" sheetId="2" r:id="rId1"/>
@@ -11905,7 +11905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
@@ -58994,8 +58994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59038,7 +59038,7 @@
         <v>28.538336000000001</v>
       </c>
       <c r="D2">
-        <v>-81.379233999999997</v>
+        <v>-81.879233999999997</v>
       </c>
       <c r="E2" s="7">
         <v>325000</v>
@@ -59064,7 +59064,7 @@
         <v>-99.174099999999996</v>
       </c>
       <c r="E3" s="7">
-        <v>1000000</v>
+        <v>750000</v>
       </c>
       <c r="F3" t="s">
         <v>3805</v>
@@ -59087,7 +59087,7 @@
         <v>134.3887</v>
       </c>
       <c r="E4" s="7">
-        <v>1000000</v>
+        <v>500000</v>
       </c>
       <c r="F4" t="s">
         <v>3805</v>
@@ -59107,7 +59107,7 @@
         <v>28.538336000000001</v>
       </c>
       <c r="D5">
-        <v>-81.379233999999997</v>
+        <v>-81.579234</v>
       </c>
       <c r="E5" s="7">
         <v>111000</v>
@@ -59130,7 +59130,7 @@
         <v>32.715736</v>
       </c>
       <c r="D6">
-        <v>-117.16108699999999</v>
+        <v>-117.66108699999999</v>
       </c>
       <c r="E6" s="7">
         <v>111000</v>
@@ -59153,7 +59153,7 @@
         <v>-35.280900000000003</v>
       </c>
       <c r="D7">
-        <v>149.13</v>
+        <v>149.63</v>
       </c>
       <c r="E7" s="7">
         <v>111000</v>
@@ -59176,7 +59176,7 @@
         <v>-28.782387</v>
       </c>
       <c r="D8">
-        <v>114.607513</v>
+        <v>114.107513</v>
       </c>
       <c r="E8" s="7">
         <v>111000</v>
@@ -59464,18 +59464,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -59593,14 +59593,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3880DD5E-8917-42BB-AA42-9F04DAC43F18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27D0860C-F54E-4E5F-9EF1-B43D49FC0784}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -59611,6 +59603,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3880DD5E-8917-42BB-AA42-9F04DAC43F18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>